<commit_message>
🏗️ Update MySQL XLSX Database
</commit_message>
<xml_diff>
--- a/examples/05-mysql/walkthrough/data.xlsx
+++ b/examples/05-mysql/walkthrough/data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipsinatra/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipsinatra/github/IDM232/examples/05-mysql/walkthrough/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982AEC55-ECB5-5D47-AF88-B7CC9CA38FD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="6420" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="20620" yWindow="6540" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Name the capture of Saddam Hussein after a movie where Americans kick ass and take names? You make the list.</t>
   </si>
@@ -60,13 +61,22 @@
   </si>
   <si>
     <t>Operation Overloard</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,6 +120,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -120,13 +133,19 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 1" descr="/var/folders/_y/0yvj5kvj6pjdttkws2bml1yw0000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/photo-1523299430930-662665409fc9?ixlib=rb-0.3.5&amp;q=80&amp;fm=jpg&amp;crop=entropy&amp;cs=tinysrgb&amp;w=640&amp;h=360&amp;fit=crop&amp;ixid=eyJhcHBfaWQiOjF9&amp;s=02936870d3303fcde4bb937e5f08ce69"/>
+        <xdr:cNvPr id="2" name="AutoShape 1" descr="/var/folders/_y/0yvj5kvj6pjdttkws2bml1yw0000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/photo-1523299430930-662665409fc9?ixlib=rb-0.3.5&amp;q=80&amp;fm=jpg&amp;crop=entropy&amp;cs=tinysrgb&amp;w=640&amp;h=360&amp;fit=crop&amp;ixid=eyJhcHBfaWQiOjF9&amp;s=02936870d3303fcde4bb937e5f08ce69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -165,13 +184,19 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2" descr="/var/folders/_y/0yvj5kvj6pjdttkws2bml1yw0000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/photo-1523299430930-662665409fc9?ixlib=rb-0.3.5&amp;q=80&amp;fm=jpg&amp;crop=entropy&amp;cs=tinysrgb&amp;w=640&amp;h=360&amp;fit=crop&amp;ixid=eyJhcHBfaWQiOjF9&amp;s=02936870d3303fcde4bb937e5f08ce69"/>
+        <xdr:cNvPr id="3" name="AutoShape 2" descr="/var/folders/_y/0yvj5kvj6pjdttkws2bml1yw0000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/photo-1523299430930-662665409fc9?ixlib=rb-0.3.5&amp;q=80&amp;fm=jpg&amp;crop=entropy&amp;cs=tinysrgb&amp;w=640&amp;h=360&amp;fit=crop&amp;ixid=eyJhcHBfaWQiOjF9&amp;s=02936870d3303fcde4bb937e5f08ce69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -471,70 +496,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="32">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="32">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="48">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>